<commit_message>
# reconstruct the whole process
</commit_message>
<xml_diff>
--- a/bestPath.xlsx
+++ b/bestPath.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simon\Documents\GitHub\sdn-with-aco\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grad-cb4101\Desktop\sdn-with-aco\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F18FC2-0A7F-4780-8C15-2AD9EEA95988}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B66D193-F078-482E-901F-B25CF9556F10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6252" yWindow="1524" windowWidth="11076" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23520" yWindow="3585" windowWidth="21600" windowHeight="10950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -334,9 +334,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>